<commit_message>
Committed after the accidental Deletion and Merger of all work files
Committed after the accidental Deletion and Merger of all work files
03/07/2023 - 1:38PM IST
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Commerce@anodiam/Scope-Commerce.xlsx
+++ b/Offline/BusinessManagement/Commerce@anodiam/Scope-Commerce.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="828" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="828" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="IX-X" sheetId="5" r:id="rId1"/>
@@ -12,15 +12,15 @@
     <sheet name="BCom" sheetId="9" r:id="rId3"/>
     <sheet name="BBA" sheetId="10" r:id="rId4"/>
     <sheet name="Professional Courses" sheetId="6" r:id="rId5"/>
-    <sheet name="Corporate Training" sheetId="7" r:id="rId6"/>
+    <sheet name="CA" sheetId="11" r:id="rId6"/>
+    <sheet name="Corporate Training" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="271">
   <si>
     <t>English</t>
   </si>
@@ -365,13 +365,649 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Sl #</t>
+  </si>
+  <si>
+    <t>Courses</t>
+  </si>
+  <si>
+    <t>Subjects</t>
+  </si>
+  <si>
+    <t>Foundation</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Levels</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Application - Case Study</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>SME - Real Life Cases</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CS-Compliance</t>
+  </si>
+  <si>
+    <t>CMA</t>
+  </si>
+  <si>
+    <t>Corporate Laws - Companies Act, GST, IT, Customs, Excise, Sale of Goods, Partnership, LLP</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>www.icai.org</t>
+  </si>
+  <si>
+    <t>www.icsi.edu</t>
+  </si>
+  <si>
+    <t>www.icmai.in</t>
+  </si>
+  <si>
+    <t>CFA (International)</t>
+  </si>
+  <si>
+    <t>www.cfainstitute.org</t>
+  </si>
+  <si>
+    <t>www.isaca.org</t>
+  </si>
+  <si>
+    <t>www.isc2.org</t>
+  </si>
+  <si>
+    <t>CISSP (US) - Certified Information Systems Security Professional</t>
+  </si>
+  <si>
+    <t>CISA (US) - Certified Information Systems Audit</t>
+  </si>
+  <si>
+    <t>Production Management</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Systems</t>
+  </si>
+  <si>
+    <t>Materials</t>
+  </si>
+  <si>
+    <t>Hospitality</t>
+  </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>XLRI / VGSoM / Symbiosis</t>
+  </si>
+  <si>
+    <t>? Faculty</t>
+  </si>
+  <si>
+    <t>Framework Institute</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Business Management (MBA)</t>
+  </si>
+  <si>
+    <t>Classroom to Boardroom</t>
+  </si>
+  <si>
+    <t>Knowledge</t>
+  </si>
+  <si>
+    <t>Employee to Manager</t>
+  </si>
+  <si>
+    <t>Team work, Domain Knowledge, Grooming, Sales Training, IT Skills (MS Office, ERP Workflow)</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Freshers</t>
+  </si>
+  <si>
+    <t>EP</t>
+  </si>
+  <si>
+    <t>Executive Training</t>
+  </si>
+  <si>
+    <t>Niche, Certification: Ashbridge UK (Anamitra Chatterjee)</t>
+  </si>
+  <si>
+    <t>Domain Knowledge, Team Building, Leadership, Soft Skills</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Fees</t>
+  </si>
+  <si>
+    <t>4Hrs</t>
+  </si>
+  <si>
+    <t>2Days</t>
+  </si>
+  <si>
+    <t>Prince2, Agile Scrum, Bullet Proof Managers</t>
+  </si>
+  <si>
+    <t>Mid Level managers</t>
+  </si>
+  <si>
+    <t>Management Methodologies</t>
+  </si>
+  <si>
+    <t>Found</t>
+  </si>
+  <si>
+    <t>classes/week</t>
+  </si>
+  <si>
+    <t>Hrs/class</t>
+  </si>
+  <si>
+    <t>Rate at once</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course Duration </t>
+  </si>
+  <si>
+    <t># of Papers</t>
+  </si>
+  <si>
+    <t>Inter</t>
+  </si>
+  <si>
+    <t>20 Wks</t>
+  </si>
+  <si>
+    <t>CFA</t>
+  </si>
+  <si>
+    <t>Ac</t>
+  </si>
+  <si>
+    <t>Corp &amp; other Laws</t>
+  </si>
+  <si>
+    <t>Cost &amp; Mgmt Ac</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
+  <si>
+    <t>Adv Ac</t>
+  </si>
+  <si>
+    <t>EIS &amp; Strategic Mgmt</t>
+  </si>
+  <si>
+    <t>Fin Mgmt &amp; Eco</t>
+  </si>
+  <si>
+    <t>Bix laws &amp; correspondence</t>
+  </si>
+  <si>
+    <t>Biz Math + Stat</t>
+  </si>
+  <si>
+    <t>Eco &amp; Comm Knowledge</t>
+  </si>
+  <si>
+    <t>Fin Reporting</t>
+  </si>
+  <si>
+    <t>Strategic Fin Management</t>
+  </si>
+  <si>
+    <t>Audit &amp; Ethics</t>
+  </si>
+  <si>
+    <t>Corporate &amp; Eco Laws</t>
+  </si>
+  <si>
+    <t>Strategic Cost Mgmt &amp; Perf Eval</t>
+  </si>
+  <si>
+    <t>Risk Mgmt, Capital Markets, International Taxation, Eco Laws, Global Fin Reporting Standards</t>
+  </si>
+  <si>
+    <t>Direct Tax laws and International Taxation</t>
+  </si>
+  <si>
+    <t>Indirect Tax laws</t>
+  </si>
+  <si>
+    <t>Bix laws &amp; comm</t>
+  </si>
+  <si>
+    <t>Fin &amp; Cost AC</t>
+  </si>
+  <si>
+    <t>Biz math &amp; Stat</t>
+  </si>
+  <si>
+    <t>Buz Eco &amp; Math</t>
+  </si>
+  <si>
+    <t>Biz Law &amp; Ethics</t>
+  </si>
+  <si>
+    <t>Fin Ac</t>
+  </si>
+  <si>
+    <t>Direct Indirect Tax</t>
+  </si>
+  <si>
+    <t>Cost AC</t>
+  </si>
+  <si>
+    <t>Ops Mgmt &amp; Strategic Management</t>
+  </si>
+  <si>
+    <t>Corporate AC &amp; Auditing</t>
+  </si>
+  <si>
+    <t>Fin Management &amp; Biz Data Analytics</t>
+  </si>
+  <si>
+    <t>Mgmt AC</t>
+  </si>
+  <si>
+    <t>Direct Tax laws &amp; International Tax laws</t>
+  </si>
+  <si>
+    <t>Strategic Cost Management</t>
+  </si>
+  <si>
+    <t>Cost &amp; Management Audit</t>
+  </si>
+  <si>
+    <t>Corporate Fin Reporting</t>
+  </si>
+  <si>
+    <t>Indirect Tax</t>
+  </si>
+  <si>
+    <t>Strategic Performance Mgmt &amp; Biz Val</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Biz Env &amp; Law</t>
+  </si>
+  <si>
+    <t>Biz Mgmt, Ethics &amp; Enterpreneurship</t>
+  </si>
+  <si>
+    <t>Bix Eco</t>
+  </si>
+  <si>
+    <t>AC &amp; Audit</t>
+  </si>
+  <si>
+    <t>General Law</t>
+  </si>
+  <si>
+    <t>Sett up of Business Entities &amp; Closure</t>
+  </si>
+  <si>
+    <t>Tax Law</t>
+  </si>
+  <si>
+    <t>Corporate &amp; Mgmt AC</t>
+  </si>
+  <si>
+    <t>Securities Law &amp; Capital Mkt</t>
+  </si>
+  <si>
+    <t>Economic, Biz &amp; Commercial Law</t>
+  </si>
+  <si>
+    <t>Financial &amp; Strategic Mgmt</t>
+  </si>
+  <si>
+    <t>Governance, Risk Mgmt &amp; Ethics</t>
+  </si>
+  <si>
+    <t>Adv Tax laws</t>
+  </si>
+  <si>
+    <t>Drafting, Pleeding &amp;Appearances</t>
+  </si>
+  <si>
+    <t>Secreterial Audit &amp; Due Delegence</t>
+  </si>
+  <si>
+    <t>Corporate Restructuring, Insolvancy &amp; Winding Up</t>
+  </si>
+  <si>
+    <t>Resolution of Corporate Disputes</t>
+  </si>
+  <si>
+    <t>Corporate Funding &amp; Stock Exchange Listing</t>
+  </si>
+  <si>
+    <t>Multi Disciplinary Case Studies</t>
+  </si>
+  <si>
+    <t>Intellectual Property Rights</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>2 hrs</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>Ethical &amp; Professional Standards</t>
+  </si>
+  <si>
+    <t>Quantitive Methods</t>
+  </si>
+  <si>
+    <t>Financial Statement Analysis</t>
+  </si>
+  <si>
+    <t>Corporate Issuers</t>
+  </si>
+  <si>
+    <t>Equity Investments</t>
+  </si>
+  <si>
+    <t>Fixed Income</t>
+  </si>
+  <si>
+    <t>Derivatives</t>
+  </si>
+  <si>
+    <t>Alternative Investments</t>
+  </si>
+  <si>
+    <t>Portrfolio Mgmt &amp; Wealth Planning</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Study Material</t>
+  </si>
+  <si>
+    <t>foundation</t>
+  </si>
+  <si>
+    <t>Paper-I (Priciples and practise of Accounting)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t xml:space="preserve">MODULE 1 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t>Theoretical Framework, Accounting Process, Bank reconcilliation statement, Inventories, Concept and accounting of Depreciation, Accounting for special Transaction</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t xml:space="preserve">MODULE 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t>- Peparation of final accounts,Partnership Accounts, Financial Statements of Not-for-Profit Organizations, Company Accounts</t>
+    </r>
+  </si>
+  <si>
+    <t>Paper-II (Business Laws and Business Coerrespondence and Reporting)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t xml:space="preserve">Sec-A Business Laws- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t xml:space="preserve">     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t>The Indian Contract Act, 1872, The Sale of Goods Act, 1930, The Indian Partnership Act, 1932, The Limited Liability Partnership Act, 2008, The Companies Act, 2013</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sec-B Business Correspondence and Reporting- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t xml:space="preserve">Communication, Sentence Types, Active-Passive Voice and Direct-Indirect Speech, Vocabulary, Comprehension Passages, Note Making, Introduction to Basics of Writing,Precis writing, Article writing,Report writing,  Formal Letters and Official Communication, Writing Formal Mails, Resume Writing,  Meetings </t>
+    </r>
+  </si>
+  <si>
+    <t>Paper-III ( Business Mathematics, Logical Reasoning Statistics)</t>
+  </si>
+  <si>
+    <r>
+      <t>Part-A Business Mathematics-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t>Ratio and Proportion, Indices, Logar, Equations, Linear Inequalities, Time Value of Money, Basic Concepts of Permutations and C, Sequence and Series - Arithmetic ,Sets, Functions and Relations, Basic Concepts of Differential and I,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Part-B Logical Reasoning- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t>Number Series, Coding and Decoding , Direction Tests,  Seating Arrangements, blood relations</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Part-C Statistics- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t xml:space="preserve"> Statistical Description of Data, Measures of Central Tendency and Dispersion, Probability,Theoretical Distributions  Index Numbers,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t>Correlation And Regression,18, Index Numbers</t>
+    </r>
+  </si>
+  <si>
+    <t>Paper-IV (Business Economics, and Business and Commercial Knowledge)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t>Part-I Business Economics</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t xml:space="preserve"> Nature &amp; Scope of Business Economic,  Theory of Demand and Supply,  Theory of Production and Cost,  Price Determination in Different Market, Business Cycles </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t xml:space="preserve">Part-II Business and Commercial Knowledge- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <rFont val="Oxygen"/>
+      </rPr>
+      <t>Business and commercial knowledge, Business Enviornment,  Business Org, Government Policies, Organizations Facilitating Business,  Common Business Terminologies</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,8 +1029,90 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Oxygen"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Oxygen"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Oxygen"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Oxygen"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Oxygen"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Oxygen"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Oxygen"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Oxygen"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Oxygen"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Oxygen"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Oxygen"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Oxygen"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Oxygen"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,8 +1179,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="39">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -958,11 +1724,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1033,6 +1873,152 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1165,8 +2151,18 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1507,7 +2503,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="114" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1522,12 +2518,12 @@
       <c r="F3" s="6">
         <v>100</v>
       </c>
-      <c r="G3" s="72" t="s">
+      <c r="G3" s="122" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="65"/>
+      <c r="B4" s="115"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -1538,10 +2534,10 @@
       <c r="F4" s="7">
         <v>100</v>
       </c>
-      <c r="G4" s="73"/>
+      <c r="G4" s="123"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="65"/>
+      <c r="B5" s="115"/>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1554,10 +2550,10 @@
       <c r="F5" s="7">
         <v>100</v>
       </c>
-      <c r="G5" s="73"/>
+      <c r="G5" s="123"/>
     </row>
     <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="66"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
         <v>8</v>
@@ -1568,10 +2564,10 @@
       <c r="F6" s="9">
         <v>100</v>
       </c>
-      <c r="G6" s="73"/>
+      <c r="G6" s="123"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="117" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -1586,10 +2582,10 @@
       <c r="F7" s="12">
         <v>20</v>
       </c>
-      <c r="G7" s="73"/>
+      <c r="G7" s="123"/>
     </row>
     <row r="8" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="68"/>
+      <c r="B8" s="118"/>
       <c r="C8" s="13" t="s">
         <v>6</v>
       </c>
@@ -1602,10 +2598,10 @@
       <c r="F8" s="14">
         <v>20</v>
       </c>
-      <c r="G8" s="73"/>
+      <c r="G8" s="123"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="119" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -1620,10 +2616,10 @@
       <c r="F9" s="16">
         <v>100</v>
       </c>
-      <c r="G9" s="73"/>
+      <c r="G9" s="123"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="70"/>
+      <c r="B10" s="120"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
         <v>11</v>
@@ -1634,10 +2630,10 @@
       <c r="F10" s="17">
         <v>100</v>
       </c>
-      <c r="G10" s="73"/>
+      <c r="G10" s="123"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="70"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1650,10 +2646,10 @@
       <c r="F11" s="17">
         <v>100</v>
       </c>
-      <c r="G11" s="73"/>
+      <c r="G11" s="123"/>
     </row>
     <row r="12" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="71"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18" t="s">
         <v>11</v>
@@ -1664,7 +2660,7 @@
       <c r="F12" s="19">
         <v>100</v>
       </c>
-      <c r="G12" s="74"/>
+      <c r="G12" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1682,8 +2678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1718,7 +2714,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="115" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="26" t="s">
@@ -1733,12 +2729,12 @@
       <c r="F3" s="27">
         <v>100</v>
       </c>
-      <c r="G3" s="72" t="s">
+      <c r="G3" s="122" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="65"/>
+      <c r="B4" s="115"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
         <v>15</v>
@@ -1749,10 +2745,10 @@
       <c r="F4" s="7">
         <v>100</v>
       </c>
-      <c r="G4" s="73"/>
+      <c r="G4" s="123"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="65"/>
+      <c r="B5" s="115"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -1763,10 +2759,10 @@
       <c r="F5" s="7">
         <v>100</v>
       </c>
-      <c r="G5" s="73"/>
+      <c r="G5" s="123"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="65"/>
+      <c r="B6" s="115"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -1777,10 +2773,10 @@
       <c r="F6" s="7">
         <v>100</v>
       </c>
-      <c r="G6" s="73"/>
+      <c r="G6" s="123"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="65"/>
+      <c r="B7" s="115"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
         <v>28</v>
@@ -1791,10 +2787,10 @@
       <c r="F7" s="7">
         <v>100</v>
       </c>
-      <c r="G7" s="73"/>
+      <c r="G7" s="123"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="65"/>
+      <c r="B8" s="115"/>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1807,10 +2803,10 @@
       <c r="F8" s="7">
         <v>100</v>
       </c>
-      <c r="G8" s="73"/>
+      <c r="G8" s="123"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="65"/>
+      <c r="B9" s="115"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
         <v>15</v>
@@ -1821,10 +2817,10 @@
       <c r="F9" s="7">
         <v>100</v>
       </c>
-      <c r="G9" s="73"/>
+      <c r="G9" s="123"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="65"/>
+      <c r="B10" s="115"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -1835,10 +2831,10 @@
       <c r="F10" s="7">
         <v>100</v>
       </c>
-      <c r="G10" s="73"/>
+      <c r="G10" s="123"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="65"/>
+      <c r="B11" s="115"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
         <v>16</v>
@@ -1849,10 +2845,10 @@
       <c r="F11" s="7">
         <v>100</v>
       </c>
-      <c r="G11" s="73"/>
+      <c r="G11" s="123"/>
     </row>
     <row r="12" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="66"/>
+      <c r="B12" s="116"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
         <v>28</v>
@@ -1863,10 +2859,10 @@
       <c r="F12" s="9">
         <v>100</v>
       </c>
-      <c r="G12" s="73"/>
+      <c r="G12" s="123"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="117" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1881,10 +2877,10 @@
       <c r="F13" s="22">
         <v>100</v>
       </c>
-      <c r="G13" s="73"/>
+      <c r="G13" s="123"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="75"/>
+      <c r="B14" s="125"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -1895,10 +2891,10 @@
       <c r="F14" s="21">
         <v>100</v>
       </c>
-      <c r="G14" s="73"/>
+      <c r="G14" s="123"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="75"/>
+      <c r="B15" s="125"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
         <v>16</v>
@@ -1909,10 +2905,10 @@
       <c r="F15" s="21">
         <v>100</v>
       </c>
-      <c r="G15" s="73"/>
+      <c r="G15" s="123"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="75"/>
+      <c r="B16" s="125"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
         <v>18</v>
@@ -1923,10 +2919,10 @@
       <c r="F16" s="21">
         <v>100</v>
       </c>
-      <c r="G16" s="73"/>
+      <c r="G16" s="123"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="75"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
         <v>19</v>
@@ -1937,10 +2933,10 @@
       <c r="F17" s="21">
         <v>100</v>
       </c>
-      <c r="G17" s="73"/>
+      <c r="G17" s="123"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="75"/>
+      <c r="B18" s="125"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
         <v>28</v>
@@ -1951,10 +2947,10 @@
       <c r="F18" s="21">
         <v>100</v>
       </c>
-      <c r="G18" s="73"/>
+      <c r="G18" s="123"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="75"/>
+      <c r="B19" s="125"/>
       <c r="C19" s="2" t="s">
         <v>13</v>
       </c>
@@ -1967,10 +2963,10 @@
       <c r="F19" s="21">
         <v>100</v>
       </c>
-      <c r="G19" s="73"/>
+      <c r="G19" s="123"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="75"/>
+      <c r="B20" s="125"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>8</v>
@@ -1981,10 +2977,10 @@
       <c r="F20" s="21">
         <v>100</v>
       </c>
-      <c r="G20" s="73"/>
+      <c r="G20" s="123"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="75"/>
+      <c r="B21" s="125"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>16</v>
@@ -1995,10 +2991,10 @@
       <c r="F21" s="21">
         <v>100</v>
       </c>
-      <c r="G21" s="73"/>
+      <c r="G21" s="123"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="75"/>
+      <c r="B22" s="125"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
         <v>18</v>
@@ -2009,10 +3005,10 @@
       <c r="F22" s="21">
         <v>100</v>
       </c>
-      <c r="G22" s="73"/>
+      <c r="G22" s="123"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="75"/>
+      <c r="B23" s="125"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>19</v>
@@ -2023,10 +3019,10 @@
       <c r="F23" s="21">
         <v>100</v>
       </c>
-      <c r="G23" s="73"/>
+      <c r="G23" s="123"/>
     </row>
     <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="68"/>
+      <c r="B24" s="118"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13" t="s">
         <v>28</v>
@@ -2037,10 +3033,10 @@
       <c r="F24" s="14">
         <v>100</v>
       </c>
-      <c r="G24" s="73"/>
+      <c r="G24" s="123"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="69" t="s">
+      <c r="B25" s="119" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="10" t="s">
@@ -2055,10 +3051,10 @@
       <c r="F25" s="20">
         <v>100</v>
       </c>
-      <c r="G25" s="73"/>
+      <c r="G25" s="123"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="70"/>
+      <c r="B26" s="120"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
         <v>8</v>
@@ -2069,10 +3065,10 @@
       <c r="F26" s="17">
         <v>100</v>
       </c>
-      <c r="G26" s="73"/>
+      <c r="G26" s="123"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="70"/>
+      <c r="B27" s="120"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
         <v>16</v>
@@ -2083,10 +3079,10 @@
       <c r="F27" s="17">
         <v>100</v>
       </c>
-      <c r="G27" s="73"/>
+      <c r="G27" s="123"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="70"/>
+      <c r="B28" s="120"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
         <v>21</v>
@@ -2097,10 +3093,10 @@
       <c r="F28" s="17">
         <v>100</v>
       </c>
-      <c r="G28" s="73"/>
+      <c r="G28" s="123"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="70"/>
+      <c r="B29" s="120"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
         <v>22</v>
@@ -2111,10 +3107,10 @@
       <c r="F29" s="17">
         <v>100</v>
       </c>
-      <c r="G29" s="73"/>
+      <c r="G29" s="123"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="70"/>
+      <c r="B30" s="120"/>
       <c r="C30" s="3" t="s">
         <v>13</v>
       </c>
@@ -2127,10 +3123,10 @@
       <c r="F30" s="17">
         <v>100</v>
       </c>
-      <c r="G30" s="73"/>
+      <c r="G30" s="123"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="70"/>
+      <c r="B31" s="120"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
         <v>8</v>
@@ -2141,10 +3137,10 @@
       <c r="F31" s="17">
         <v>100</v>
       </c>
-      <c r="G31" s="73"/>
+      <c r="G31" s="123"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="70"/>
+      <c r="B32" s="120"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
         <v>16</v>
@@ -2155,10 +3151,10 @@
       <c r="F32" s="17">
         <v>100</v>
       </c>
-      <c r="G32" s="73"/>
+      <c r="G32" s="123"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="70"/>
+      <c r="B33" s="120"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
         <v>21</v>
@@ -2169,10 +3165,10 @@
       <c r="F33" s="17">
         <v>100</v>
       </c>
-      <c r="G33" s="73"/>
+      <c r="G33" s="123"/>
     </row>
     <row r="34" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="71"/>
+      <c r="B34" s="121"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18" t="s">
         <v>22</v>
@@ -2183,7 +3179,7 @@
       <c r="F34" s="19">
         <v>100</v>
       </c>
-      <c r="G34" s="74"/>
+      <c r="G34" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2201,8 +3197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H28"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2239,155 +3235,155 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="132" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="134" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="123" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="73" t="s">
+      <c r="F3" s="123" t="s">
         <v>71</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="72" t="s">
+      <c r="H3" s="122" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="82"/>
+      <c r="B4" s="132"/>
       <c r="C4" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
       <c r="G4" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="73"/>
+      <c r="H4" s="123"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="82"/>
+      <c r="B5" s="132"/>
       <c r="C5" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="82"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
+      <c r="D5" s="132"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
       <c r="G5" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="73"/>
+      <c r="H5" s="123"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="82"/>
+      <c r="B6" s="132"/>
       <c r="C6" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
       <c r="G6" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="73"/>
+      <c r="H6" s="123"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="82"/>
+      <c r="B7" s="132"/>
       <c r="C7" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="82"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="123"/>
       <c r="G7" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="73"/>
+      <c r="H7" s="123"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="82"/>
+      <c r="B8" s="132"/>
       <c r="C8" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="82"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
       <c r="G8" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="73"/>
+      <c r="H8" s="123"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="82"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
       <c r="G9" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="73"/>
+      <c r="H9" s="123"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="82"/>
+      <c r="B10" s="132"/>
       <c r="C10" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="82"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
       <c r="G10" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="73"/>
+      <c r="H10" s="123"/>
     </row>
     <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="82"/>
+      <c r="B11" s="132"/>
       <c r="C11" s="36"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
       <c r="G11" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="H11" s="73"/>
+      <c r="H11" s="123"/>
     </row>
     <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="83"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="73"/>
+      <c r="B12" s="133"/>
+      <c r="D12" s="132"/>
+      <c r="E12" s="124"/>
+      <c r="F12" s="123"/>
       <c r="G12" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="H12" s="74"/>
+      <c r="H12" s="124"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="82"/>
-      <c r="E13" s="85" t="s">
+      <c r="D13" s="132"/>
+      <c r="E13" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="76" t="s">
+      <c r="F13" s="126" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="88" t="s">
+      <c r="H13" s="138" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2395,39 +3391,39 @@
       <c r="B14" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="82"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="77"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="136"/>
+      <c r="F14" s="127"/>
       <c r="G14" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="89"/>
+      <c r="H14" s="139"/>
     </row>
     <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="82"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="78"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="136"/>
+      <c r="F15" s="128"/>
       <c r="G15" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="90"/>
+      <c r="H15" s="140"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="82"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="98" t="s">
+      <c r="D16" s="132"/>
+      <c r="E16" s="136"/>
+      <c r="F16" s="148" t="s">
         <v>62</v>
       </c>
       <c r="G16" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="91" t="s">
+      <c r="H16" s="141" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2435,100 +3431,100 @@
       <c r="B17" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="82"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="99"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="136"/>
+      <c r="F17" s="149"/>
       <c r="G17" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="92"/>
+      <c r="H17" s="142"/>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="82"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="100"/>
+      <c r="D18" s="132"/>
+      <c r="E18" s="136"/>
+      <c r="F18" s="150"/>
       <c r="G18" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="H18" s="93"/>
+      <c r="H18" s="143"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="82"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="104" t="s">
+      <c r="D19" s="132"/>
+      <c r="E19" s="136"/>
+      <c r="F19" s="154" t="s">
         <v>65</v>
       </c>
       <c r="G19" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="79" t="s">
+      <c r="H19" s="129" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="33"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="105"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="136"/>
+      <c r="F20" s="155"/>
       <c r="G20" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="H20" s="80"/>
+      <c r="H20" s="130"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D21" s="82"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="106" t="s">
+      <c r="D21" s="132"/>
+      <c r="E21" s="136"/>
+      <c r="F21" s="156" t="s">
         <v>67</v>
       </c>
       <c r="G21" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="94" t="s">
+      <c r="H21" s="144" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D22" s="82"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="107"/>
+      <c r="D22" s="132"/>
+      <c r="E22" s="136"/>
+      <c r="F22" s="157"/>
       <c r="G22" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="H22" s="95"/>
+      <c r="H22" s="145"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D23" s="82"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="101" t="s">
+      <c r="D23" s="132"/>
+      <c r="E23" s="136"/>
+      <c r="F23" s="151" t="s">
         <v>70</v>
       </c>
       <c r="G23" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="H23" s="96" t="s">
+      <c r="H23" s="146" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D24" s="82"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="102"/>
+      <c r="D24" s="132"/>
+      <c r="E24" s="136"/>
+      <c r="F24" s="152"/>
       <c r="G24" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="H24" s="97"/>
+      <c r="H24" s="147"/>
     </row>
     <row r="25" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D25" s="82"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="102"/>
+      <c r="D25" s="132"/>
+      <c r="E25" s="136"/>
+      <c r="F25" s="152"/>
       <c r="G25" s="51" t="s">
         <v>74</v>
       </c>
@@ -2537,33 +3533,33 @@
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D26" s="82"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="102"/>
+      <c r="D26" s="132"/>
+      <c r="E26" s="136"/>
+      <c r="F26" s="152"/>
       <c r="G26" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="H26" s="79" t="s">
+      <c r="H26" s="129" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D27" s="82"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="102"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="136"/>
+      <c r="F27" s="152"/>
       <c r="G27" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="H27" s="81"/>
+      <c r="H27" s="131"/>
     </row>
     <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D28" s="83"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="103"/>
+      <c r="D28" s="133"/>
+      <c r="E28" s="137"/>
+      <c r="F28" s="153"/>
       <c r="G28" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="H28" s="80"/>
+      <c r="H28" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -2595,7 +3591,7 @@
   <dimension ref="B1:F32"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F32"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2624,74 +3620,74 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="132" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="132" t="s">
         <v>47</v>
       </c>
       <c r="E3" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="79" t="s">
+      <c r="F3" s="129" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="82"/>
+      <c r="B4" s="132"/>
       <c r="C4" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="82"/>
+      <c r="D4" s="132"/>
       <c r="E4" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="80"/>
+      <c r="F4" s="130"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="82"/>
+      <c r="B5" s="132"/>
       <c r="C5" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="82"/>
+      <c r="D5" s="132"/>
       <c r="E5" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="79" t="s">
+      <c r="F5" s="129" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="82"/>
+      <c r="B6" s="132"/>
       <c r="C6" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="82"/>
+      <c r="D6" s="132"/>
       <c r="E6" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="81"/>
+      <c r="F6" s="131"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="82"/>
+      <c r="B7" s="132"/>
       <c r="C7" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="82"/>
+      <c r="D7" s="132"/>
       <c r="E7" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="80"/>
+      <c r="F7" s="130"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="82"/>
+      <c r="B8" s="132"/>
       <c r="C8" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="82"/>
+      <c r="D8" s="132"/>
       <c r="E8" s="61" t="s">
         <v>87</v>
       </c>
@@ -2700,210 +3696,210 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="82"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="82"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="122" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="82"/>
+      <c r="B10" s="132"/>
       <c r="C10" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="82"/>
+      <c r="D10" s="132"/>
       <c r="E10" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="73"/>
+      <c r="F10" s="123"/>
     </row>
     <row r="11" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="82"/>
+      <c r="B11" s="132"/>
       <c r="C11" s="36"/>
-      <c r="D11" s="82"/>
+      <c r="D11" s="132"/>
       <c r="E11" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="F11" s="73"/>
+      <c r="F11" s="123"/>
     </row>
     <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="83"/>
-      <c r="D12" s="82"/>
+      <c r="B12" s="133"/>
+      <c r="D12" s="132"/>
       <c r="E12" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="F12" s="73"/>
+      <c r="F12" s="123"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="82"/>
+      <c r="D13" s="132"/>
       <c r="E13" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="F13" s="73"/>
+      <c r="F13" s="123"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="82"/>
+      <c r="D14" s="132"/>
       <c r="E14" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="73"/>
+      <c r="F14" s="123"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="82"/>
+      <c r="D15" s="132"/>
       <c r="E15" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="73"/>
+      <c r="F15" s="123"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="82"/>
+      <c r="D16" s="132"/>
       <c r="E16" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="73"/>
+      <c r="F16" s="123"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="82"/>
+      <c r="D17" s="132"/>
       <c r="E17" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="73"/>
+      <c r="F17" s="123"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="82"/>
+      <c r="D18" s="132"/>
       <c r="E18" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="73"/>
+      <c r="F18" s="123"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="82"/>
+      <c r="D19" s="132"/>
       <c r="E19" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="73"/>
+      <c r="F19" s="123"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="82"/>
+      <c r="D20" s="132"/>
       <c r="E20" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="F20" s="73"/>
+      <c r="F20" s="123"/>
     </row>
     <row r="21" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="33"/>
-      <c r="D21" s="82"/>
+      <c r="D21" s="132"/>
       <c r="E21" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="73"/>
+      <c r="F21" s="123"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D22" s="82"/>
+      <c r="D22" s="132"/>
       <c r="E22" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="F22" s="73"/>
+      <c r="F22" s="123"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D23" s="82"/>
+      <c r="D23" s="132"/>
       <c r="E23" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="73"/>
+      <c r="F23" s="123"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D24" s="82"/>
+      <c r="D24" s="132"/>
       <c r="E24" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="F24" s="73"/>
+      <c r="F24" s="123"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D25" s="82"/>
+      <c r="D25" s="132"/>
       <c r="E25" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="73"/>
+      <c r="F25" s="123"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D26" s="82"/>
+      <c r="D26" s="132"/>
       <c r="E26" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="F26" s="73"/>
+      <c r="F26" s="123"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D27" s="82"/>
+      <c r="D27" s="132"/>
       <c r="E27" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="F27" s="73"/>
+      <c r="F27" s="123"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D28" s="82"/>
+      <c r="D28" s="132"/>
       <c r="E28" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="F28" s="73"/>
+      <c r="F28" s="123"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D29" s="82"/>
+      <c r="D29" s="132"/>
       <c r="E29" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="73"/>
+      <c r="F29" s="123"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D30" s="82"/>
+      <c r="D30" s="132"/>
       <c r="E30" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="73"/>
+      <c r="F30" s="123"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D31" s="82"/>
+      <c r="D31" s="132"/>
       <c r="E31" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="73"/>
+      <c r="F31" s="123"/>
     </row>
     <row r="32" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D32" s="83"/>
+      <c r="D32" s="133"/>
       <c r="E32" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="F32" s="74"/>
+      <c r="F32" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2920,24 +3916,1399 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:T54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="3.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.109375" style="64" customWidth="1"/>
+    <col min="2" max="2" width="3.88671875" style="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.44140625" style="64" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="64" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.77734375" style="64" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="64"/>
+    <col min="8" max="8" width="4.88671875" style="64" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" style="64" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="64" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" style="64" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" style="64" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" style="64" customWidth="1"/>
+    <col min="15" max="15" width="16.88671875" style="64" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" style="64" customWidth="1"/>
+    <col min="17" max="17" width="13.5546875" style="64" customWidth="1"/>
+    <col min="18" max="20" width="14.6640625" style="64" customWidth="1"/>
+    <col min="21" max="16384" width="3.6640625" style="64"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B1" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="70" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B2" s="71">
+        <v>1</v>
+      </c>
+      <c r="C2" s="72" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="73" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="71" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B3" s="71">
+        <v>2</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="71" t="s">
+        <v>123</v>
+      </c>
+      <c r="J3" s="64" t="s">
+        <v>176</v>
+      </c>
+      <c r="K3" s="64" t="s">
+        <v>174</v>
+      </c>
+      <c r="L3" s="64" t="s">
+        <v>172</v>
+      </c>
+      <c r="M3" s="64" t="s">
+        <v>173</v>
+      </c>
+      <c r="N3" s="64" t="s">
+        <v>238</v>
+      </c>
+      <c r="O3" s="64" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="71">
+        <v>3</v>
+      </c>
+      <c r="C4" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" s="71" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" s="64" t="s">
+        <v>171</v>
+      </c>
+      <c r="J4" s="64">
+        <v>4</v>
+      </c>
+      <c r="K4" s="64">
+        <v>15</v>
+      </c>
+      <c r="L4" s="64">
+        <v>4</v>
+      </c>
+      <c r="M4" s="64">
+        <v>3</v>
+      </c>
+      <c r="N4" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="O4" s="64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B5" s="71">
+        <v>4</v>
+      </c>
+      <c r="C5" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="73" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="I5" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="J5" s="64">
+        <v>8</v>
+      </c>
+      <c r="K5" s="64">
+        <v>20</v>
+      </c>
+      <c r="L5" s="64">
+        <v>4</v>
+      </c>
+      <c r="M5" s="64">
+        <v>3</v>
+      </c>
+      <c r="N5" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="O5" s="64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B6" s="71">
+        <v>5</v>
+      </c>
+      <c r="C6" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="I6" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="64">
+        <v>8</v>
+      </c>
+      <c r="K6" s="64">
+        <v>25</v>
+      </c>
+      <c r="L6" s="64">
+        <v>4</v>
+      </c>
+      <c r="M6" s="64">
+        <v>3</v>
+      </c>
+      <c r="N6" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="O6" s="64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="71">
+        <v>6</v>
+      </c>
+      <c r="C7" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="H7" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="I7" s="64" t="s">
+        <v>171</v>
+      </c>
+      <c r="J7" s="64">
+        <v>4</v>
+      </c>
+      <c r="K7" s="64">
+        <v>15</v>
+      </c>
+      <c r="L7" s="64">
+        <v>4</v>
+      </c>
+      <c r="M7" s="64">
+        <v>3</v>
+      </c>
+      <c r="N7" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="O7" s="64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="68" t="s">
+        <v>151</v>
+      </c>
+      <c r="I8" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="J8" s="64">
+        <v>8</v>
+      </c>
+      <c r="K8" s="64">
+        <v>20</v>
+      </c>
+      <c r="L8" s="64">
+        <v>4</v>
+      </c>
+      <c r="M8" s="64">
+        <v>3</v>
+      </c>
+      <c r="N8" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="O8" s="64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="74">
+        <v>7</v>
+      </c>
+      <c r="C9" s="74" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="74" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="I9" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="J9" s="64">
+        <v>8</v>
+      </c>
+      <c r="K9" s="64">
+        <v>25</v>
+      </c>
+      <c r="L9" s="64">
+        <v>4</v>
+      </c>
+      <c r="M9" s="64">
+        <v>3</v>
+      </c>
+      <c r="N9" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="O9" s="64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="74"/>
+      <c r="H10" s="64" t="s">
+        <v>217</v>
+      </c>
+      <c r="I10" s="64" t="s">
+        <v>171</v>
+      </c>
+      <c r="J10" s="64">
+        <v>4</v>
+      </c>
+      <c r="K10" s="64">
+        <v>15</v>
+      </c>
+      <c r="L10" s="64">
+        <v>4</v>
+      </c>
+      <c r="M10" s="64">
+        <v>3</v>
+      </c>
+      <c r="N10" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="O10" s="64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74" t="s">
+        <v>142</v>
+      </c>
+      <c r="E11" s="74"/>
+      <c r="I11" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="J11" s="64">
+        <v>8</v>
+      </c>
+      <c r="K11" s="64">
+        <v>20</v>
+      </c>
+      <c r="L11" s="64">
+        <v>4</v>
+      </c>
+      <c r="M11" s="64">
+        <v>3</v>
+      </c>
+      <c r="N11" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="O11" s="64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" s="74"/>
+      <c r="I12" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="J12" s="64">
+        <v>9</v>
+      </c>
+      <c r="K12" s="64">
+        <v>25</v>
+      </c>
+      <c r="L12" s="64">
+        <v>4</v>
+      </c>
+      <c r="M12" s="64">
+        <v>3</v>
+      </c>
+      <c r="N12" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="O12" s="64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="74"/>
+      <c r="H13" s="64" t="s">
+        <v>179</v>
+      </c>
+      <c r="I13" s="64" t="s">
+        <v>243</v>
+      </c>
+      <c r="J13" s="64">
+        <v>10</v>
+      </c>
+      <c r="K13" s="64">
+        <v>25</v>
+      </c>
+      <c r="L13" s="64">
+        <v>4</v>
+      </c>
+      <c r="M13" s="64">
+        <v>3</v>
+      </c>
+      <c r="N13" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="O13" s="64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="74"/>
+      <c r="I14" s="64" t="s">
+        <v>244</v>
+      </c>
+      <c r="J14" s="64">
+        <v>10</v>
+      </c>
+      <c r="K14" s="64">
+        <v>30</v>
+      </c>
+      <c r="L14" s="64">
+        <v>4</v>
+      </c>
+      <c r="M14" s="64">
+        <v>3</v>
+      </c>
+      <c r="N14" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="O14" s="64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="E15" s="74"/>
+      <c r="I15" s="64" t="s">
+        <v>245</v>
+      </c>
+      <c r="J15" s="64">
+        <v>10</v>
+      </c>
+      <c r="K15" s="64">
+        <v>35</v>
+      </c>
+      <c r="L15" s="64">
+        <v>4</v>
+      </c>
+      <c r="M15" s="64">
+        <v>3</v>
+      </c>
+      <c r="N15" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="O15" s="64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" s="74"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17" s="74"/>
+    </row>
+    <row r="18" spans="2:20" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="74">
+        <v>8</v>
+      </c>
+      <c r="C18" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="75" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="75" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="I19" s="83" t="s">
+        <v>126</v>
+      </c>
+      <c r="J19" s="84"/>
+      <c r="K19" s="85"/>
+      <c r="L19" s="83" t="s">
+        <v>128</v>
+      </c>
+      <c r="M19" s="84"/>
+      <c r="N19" s="85"/>
+      <c r="O19" s="83" t="s">
+        <v>217</v>
+      </c>
+      <c r="P19" s="84"/>
+      <c r="Q19" s="85"/>
+      <c r="R19" s="76" t="s">
+        <v>179</v>
+      </c>
+      <c r="S19" s="77"/>
+      <c r="T19" s="78"/>
+    </row>
+    <row r="20" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
+      <c r="I20" s="86" t="s">
+        <v>171</v>
+      </c>
+      <c r="J20" s="87" t="s">
+        <v>177</v>
+      </c>
+      <c r="K20" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="L20" s="86" t="s">
+        <v>171</v>
+      </c>
+      <c r="M20" s="87" t="s">
+        <v>177</v>
+      </c>
+      <c r="N20" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="O20" s="86" t="s">
+        <v>171</v>
+      </c>
+      <c r="P20" s="87" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q20" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="R20" s="80" t="s">
+        <v>240</v>
+      </c>
+      <c r="S20" s="81" t="s">
+        <v>241</v>
+      </c>
+      <c r="T20" s="82" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B21" s="66"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="I21" s="89" t="s">
+        <v>180</v>
+      </c>
+      <c r="J21" s="90" t="s">
+        <v>180</v>
+      </c>
+      <c r="K21" s="91" t="s">
+        <v>191</v>
+      </c>
+      <c r="L21" s="89" t="s">
+        <v>199</v>
+      </c>
+      <c r="M21" s="92" t="s">
+        <v>203</v>
+      </c>
+      <c r="N21" s="93" t="s">
+        <v>194</v>
+      </c>
+      <c r="O21" s="94" t="s">
+        <v>218</v>
+      </c>
+      <c r="P21" s="92" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q21" s="93" t="s">
+        <v>229</v>
+      </c>
+      <c r="R21" s="79" t="s">
+        <v>246</v>
+      </c>
+      <c r="S21" s="79" t="s">
+        <v>246</v>
+      </c>
+      <c r="T21" s="79" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="I22" s="89" t="s">
+        <v>188</v>
+      </c>
+      <c r="J22" s="92" t="s">
+        <v>181</v>
+      </c>
+      <c r="K22" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="L22" s="89" t="s">
+        <v>200</v>
+      </c>
+      <c r="M22" s="90" t="s">
+        <v>204</v>
+      </c>
+      <c r="N22" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="O22" s="94" t="s">
+        <v>219</v>
+      </c>
+      <c r="P22" s="92" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q22" s="93" t="s">
+        <v>230</v>
+      </c>
+      <c r="R22" s="79" t="s">
+        <v>247</v>
+      </c>
+      <c r="S22" s="79" t="s">
+        <v>247</v>
+      </c>
+      <c r="T22" s="79" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="I23" s="89" t="s">
+        <v>189</v>
+      </c>
+      <c r="J23" s="90" t="s">
+        <v>182</v>
+      </c>
+      <c r="K23" s="93" t="s">
+        <v>193</v>
+      </c>
+      <c r="L23" s="89" t="s">
+        <v>201</v>
+      </c>
+      <c r="M23" s="90" t="s">
+        <v>205</v>
+      </c>
+      <c r="N23" s="91" t="s">
+        <v>211</v>
+      </c>
+      <c r="O23" s="94" t="s">
+        <v>220</v>
+      </c>
+      <c r="P23" s="92" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q23" s="93" t="s">
+        <v>231</v>
+      </c>
+      <c r="R23" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="S23" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="T23" s="79" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="I24" s="89" t="s">
+        <v>190</v>
+      </c>
+      <c r="J24" s="90" t="s">
+        <v>183</v>
+      </c>
+      <c r="K24" s="93" t="s">
+        <v>194</v>
+      </c>
+      <c r="L24" s="89" t="s">
+        <v>202</v>
+      </c>
+      <c r="M24" s="90" t="s">
+        <v>206</v>
+      </c>
+      <c r="N24" s="91" t="s">
+        <v>212</v>
+      </c>
+      <c r="O24" s="94" t="s">
+        <v>221</v>
+      </c>
+      <c r="P24" s="92" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q24" s="93" t="s">
+        <v>232</v>
+      </c>
+      <c r="R24" s="79" t="s">
+        <v>248</v>
+      </c>
+      <c r="S24" s="79" t="s">
+        <v>248</v>
+      </c>
+      <c r="T24" s="79" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="66"/>
+      <c r="I25" s="98"/>
+      <c r="J25" s="92" t="s">
+        <v>184</v>
+      </c>
+      <c r="K25" s="91" t="s">
+        <v>195</v>
+      </c>
+      <c r="L25" s="98"/>
+      <c r="M25" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="N25" s="95" t="s">
+        <v>213</v>
+      </c>
+      <c r="O25" s="98"/>
+      <c r="P25" s="92" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q25" s="93" t="s">
+        <v>233</v>
+      </c>
+      <c r="R25" s="79" t="s">
+        <v>249</v>
+      </c>
+      <c r="S25" s="79" t="s">
+        <v>249</v>
+      </c>
+      <c r="T25" s="79" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B26" s="66"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="66"/>
+      <c r="I26" s="98"/>
+      <c r="J26" s="90" t="s">
+        <v>185</v>
+      </c>
+      <c r="K26" s="93" t="s">
+        <v>196</v>
+      </c>
+      <c r="L26" s="98"/>
+      <c r="M26" s="90" t="s">
+        <v>208</v>
+      </c>
+      <c r="N26" s="91" t="s">
+        <v>214</v>
+      </c>
+      <c r="O26" s="98"/>
+      <c r="P26" s="92" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q26" s="93" t="s">
+        <v>234</v>
+      </c>
+      <c r="R26" s="79" t="s">
+        <v>250</v>
+      </c>
+      <c r="S26" s="79" t="s">
+        <v>250</v>
+      </c>
+      <c r="T26" s="79" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="I27" s="98"/>
+      <c r="J27" s="92" t="s">
+        <v>186</v>
+      </c>
+      <c r="K27" s="91" t="s">
+        <v>197</v>
+      </c>
+      <c r="L27" s="98"/>
+      <c r="M27" s="90" t="s">
+        <v>209</v>
+      </c>
+      <c r="N27" s="91" t="s">
+        <v>215</v>
+      </c>
+      <c r="O27" s="98"/>
+      <c r="P27" s="92" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q27" s="93" t="s">
+        <v>235</v>
+      </c>
+      <c r="R27" s="79" t="s">
+        <v>251</v>
+      </c>
+      <c r="S27" s="79" t="s">
+        <v>251</v>
+      </c>
+      <c r="T27" s="79" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="I28" s="99"/>
+      <c r="J28" s="96" t="s">
+        <v>187</v>
+      </c>
+      <c r="K28" s="97" t="s">
+        <v>198</v>
+      </c>
+      <c r="L28" s="99"/>
+      <c r="M28" s="96" t="s">
+        <v>210</v>
+      </c>
+      <c r="N28" s="97" t="s">
+        <v>216</v>
+      </c>
+      <c r="O28" s="99"/>
+      <c r="P28" s="87" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q28" s="88" t="s">
+        <v>236</v>
+      </c>
+      <c r="R28" s="80" t="s">
+        <v>252</v>
+      </c>
+      <c r="S28" s="80" t="s">
+        <v>252</v>
+      </c>
+      <c r="T28" s="80" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="Q29" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="R29" s="64" t="s">
+        <v>253</v>
+      </c>
+      <c r="S29" s="64" t="s">
+        <v>253</v>
+      </c>
+      <c r="T29" s="64" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="R30" s="64" t="s">
+        <v>254</v>
+      </c>
+      <c r="S30" s="64" t="s">
+        <v>254</v>
+      </c>
+      <c r="T30" s="64" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B32" s="66"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="66"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="66"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="66"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="66"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="66"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37" s="66"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="66"/>
+      <c r="C39" s="66"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="66"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="66"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="66"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="66"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="66"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44" s="66"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="66"/>
+      <c r="F44" s="66"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="66"/>
+      <c r="C45" s="66"/>
+      <c r="D45" s="66"/>
+      <c r="E45" s="66"/>
+      <c r="F45" s="66"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46" s="66"/>
+      <c r="C46" s="66"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="66"/>
+      <c r="F46" s="66"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47" s="66"/>
+      <c r="C47" s="66"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="66"/>
+      <c r="F47" s="66"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48" s="66"/>
+      <c r="C48" s="66"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="66"/>
+      <c r="F48" s="66"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B49" s="66"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="66"/>
+      <c r="F49" s="66"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B50" s="66"/>
+      <c r="C50" s="66"/>
+      <c r="D50" s="66"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="66"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" s="66"/>
+      <c r="C51" s="66"/>
+      <c r="D51" s="66"/>
+      <c r="E51" s="66"/>
+      <c r="F51" s="66"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" s="66"/>
+      <c r="C52" s="66"/>
+      <c r="D52" s="66"/>
+      <c r="E52" s="66"/>
+      <c r="F52" s="66"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="66"/>
+      <c r="C53" s="66"/>
+      <c r="D53" s="66"/>
+      <c r="E53" s="66"/>
+      <c r="F53" s="66"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="66"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="66"/>
+      <c r="E54" s="66"/>
+      <c r="F54" s="66"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" style="100" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="100" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" style="100" customWidth="1"/>
+    <col min="4" max="4" width="31.88671875" style="100" customWidth="1"/>
+    <col min="5" max="5" width="32.5546875" style="100" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="100" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="100"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="158" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="158" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="158" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="158" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+    </row>
+    <row r="2" spans="1:6" s="101" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="158"/>
+      <c r="B2" s="158"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+    </row>
+    <row r="3" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="159" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="160" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="103" t="s">
+        <v>259</v>
+      </c>
+      <c r="E3" s="104" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" s="105"/>
+    </row>
+    <row r="4" spans="1:6" ht="182.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="159"/>
+      <c r="B4" s="160"/>
+      <c r="C4" s="106" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="107" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" s="108" t="s">
+        <v>263</v>
+      </c>
+      <c r="F4" s="105"/>
+    </row>
+    <row r="5" spans="1:6" ht="126" x14ac:dyDescent="0.3">
+      <c r="A5" s="159"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="102" t="s">
+        <v>264</v>
+      </c>
+      <c r="D5" s="109" t="s">
+        <v>265</v>
+      </c>
+      <c r="E5" s="110" t="s">
+        <v>266</v>
+      </c>
+      <c r="F5" s="109" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="99.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="159"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="106" t="s">
+        <v>268</v>
+      </c>
+      <c r="D6" s="111" t="s">
+        <v>269</v>
+      </c>
+      <c r="E6" s="112" t="s">
+        <v>270</v>
+      </c>
+      <c r="F6" s="105"/>
+    </row>
+    <row r="7" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="113"/>
+    </row>
+    <row r="8" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="113"/>
+    </row>
+    <row r="9" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="113"/>
+    </row>
+    <row r="10" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="113"/>
+    </row>
+    <row r="11" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="113"/>
+    </row>
+    <row r="12" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="113"/>
+    </row>
+    <row r="13" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="113"/>
+    </row>
+    <row r="14" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="113"/>
+    </row>
+    <row r="15" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="113"/>
+    </row>
+    <row r="16" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="113"/>
+    </row>
+    <row r="17" spans="1:1" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="113"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:F2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B7:B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F4">
+        <v>10000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F5">
+        <v>25000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
some changes in ca file
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Commerce@anodiam/Scope-Commerce.xlsx
+++ b/Offline/BusinessManagement/Commerce@anodiam/Scope-Commerce.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="828" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="828" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="IX-X" sheetId="5" r:id="rId1"/>
@@ -1982,9 +1982,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2159,6 +2156,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2471,18 +2471,18 @@
       <selection activeCell="G3" sqref="G3:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
@@ -2502,8 +2502,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="114" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="113" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -2518,12 +2518,12 @@
       <c r="F3" s="6">
         <v>100</v>
       </c>
-      <c r="G3" s="122" t="s">
+      <c r="G3" s="121" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="115"/>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="114"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -2534,10 +2534,10 @@
       <c r="F4" s="7">
         <v>100</v>
       </c>
-      <c r="G4" s="123"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="115"/>
+      <c r="G4" s="122"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="114"/>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2550,10 +2550,10 @@
       <c r="F5" s="7">
         <v>100</v>
       </c>
-      <c r="G5" s="123"/>
-    </row>
-    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="116"/>
+      <c r="G5" s="122"/>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="115"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
         <v>8</v>
@@ -2564,10 +2564,10 @@
       <c r="F6" s="9">
         <v>100</v>
       </c>
-      <c r="G6" s="123"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="117" t="s">
+      <c r="G6" s="122"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="116" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -2582,10 +2582,10 @@
       <c r="F7" s="12">
         <v>20</v>
       </c>
-      <c r="G7" s="123"/>
-    </row>
-    <row r="8" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="118"/>
+      <c r="G7" s="122"/>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="117"/>
       <c r="C8" s="13" t="s">
         <v>6</v>
       </c>
@@ -2598,10 +2598,10 @@
       <c r="F8" s="14">
         <v>20</v>
       </c>
-      <c r="G8" s="123"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="119" t="s">
+      <c r="G8" s="122"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="118" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -2616,10 +2616,10 @@
       <c r="F9" s="16">
         <v>100</v>
       </c>
-      <c r="G9" s="123"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="120"/>
+      <c r="G9" s="122"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="119"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
         <v>11</v>
@@ -2630,10 +2630,10 @@
       <c r="F10" s="17">
         <v>100</v>
       </c>
-      <c r="G10" s="123"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="120"/>
+      <c r="G10" s="122"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="119"/>
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
@@ -2646,10 +2646,10 @@
       <c r="F11" s="17">
         <v>100</v>
       </c>
-      <c r="G11" s="123"/>
-    </row>
-    <row r="12" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="121"/>
+      <c r="G11" s="122"/>
+    </row>
+    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="120"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18" t="s">
         <v>11</v>
@@ -2660,7 +2660,7 @@
       <c r="F12" s="19">
         <v>100</v>
       </c>
-      <c r="G12" s="124"/>
+      <c r="G12" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2682,18 +2682,18 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
@@ -2713,8 +2713,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="115" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="114" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="26" t="s">
@@ -2729,12 +2729,12 @@
       <c r="F3" s="27">
         <v>100</v>
       </c>
-      <c r="G3" s="122" t="s">
+      <c r="G3" s="121" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="115"/>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="114"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
         <v>15</v>
@@ -2745,10 +2745,10 @@
       <c r="F4" s="7">
         <v>100</v>
       </c>
-      <c r="G4" s="123"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="115"/>
+      <c r="G4" s="122"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="114"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -2759,10 +2759,10 @@
       <c r="F5" s="7">
         <v>100</v>
       </c>
-      <c r="G5" s="123"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="115"/>
+      <c r="G5" s="122"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="114"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -2773,10 +2773,10 @@
       <c r="F6" s="7">
         <v>100</v>
       </c>
-      <c r="G6" s="123"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="115"/>
+      <c r="G6" s="122"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="114"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
         <v>28</v>
@@ -2787,10 +2787,10 @@
       <c r="F7" s="7">
         <v>100</v>
       </c>
-      <c r="G7" s="123"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="115"/>
+      <c r="G7" s="122"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="114"/>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
@@ -2803,10 +2803,10 @@
       <c r="F8" s="7">
         <v>100</v>
       </c>
-      <c r="G8" s="123"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="115"/>
+      <c r="G8" s="122"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="114"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
         <v>15</v>
@@ -2817,10 +2817,10 @@
       <c r="F9" s="7">
         <v>100</v>
       </c>
-      <c r="G9" s="123"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="115"/>
+      <c r="G9" s="122"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="114"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -2831,10 +2831,10 @@
       <c r="F10" s="7">
         <v>100</v>
       </c>
-      <c r="G10" s="123"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="115"/>
+      <c r="G10" s="122"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="114"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
         <v>16</v>
@@ -2845,10 +2845,10 @@
       <c r="F11" s="7">
         <v>100</v>
       </c>
-      <c r="G11" s="123"/>
-    </row>
-    <row r="12" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="116"/>
+      <c r="G11" s="122"/>
+    </row>
+    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="115"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
         <v>28</v>
@@ -2859,10 +2859,10 @@
       <c r="F12" s="9">
         <v>100</v>
       </c>
-      <c r="G12" s="123"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="117" t="s">
+      <c r="G12" s="122"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="116" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -2877,10 +2877,10 @@
       <c r="F13" s="22">
         <v>100</v>
       </c>
-      <c r="G13" s="123"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="125"/>
+      <c r="G13" s="122"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="124"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -2891,10 +2891,10 @@
       <c r="F14" s="21">
         <v>100</v>
       </c>
-      <c r="G14" s="123"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="125"/>
+      <c r="G14" s="122"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="124"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
         <v>16</v>
@@ -2905,10 +2905,10 @@
       <c r="F15" s="21">
         <v>100</v>
       </c>
-      <c r="G15" s="123"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="125"/>
+      <c r="G15" s="122"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="124"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
         <v>18</v>
@@ -2919,10 +2919,10 @@
       <c r="F16" s="21">
         <v>100</v>
       </c>
-      <c r="G16" s="123"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="125"/>
+      <c r="G16" s="122"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="124"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
         <v>19</v>
@@ -2933,10 +2933,10 @@
       <c r="F17" s="21">
         <v>100</v>
       </c>
-      <c r="G17" s="123"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="125"/>
+      <c r="G17" s="122"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="124"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
         <v>28</v>
@@ -2947,10 +2947,10 @@
       <c r="F18" s="21">
         <v>100</v>
       </c>
-      <c r="G18" s="123"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="125"/>
+      <c r="G18" s="122"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="124"/>
       <c r="C19" s="2" t="s">
         <v>13</v>
       </c>
@@ -2963,10 +2963,10 @@
       <c r="F19" s="21">
         <v>100</v>
       </c>
-      <c r="G19" s="123"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="125"/>
+      <c r="G19" s="122"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="124"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>8</v>
@@ -2977,10 +2977,10 @@
       <c r="F20" s="21">
         <v>100</v>
       </c>
-      <c r="G20" s="123"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="125"/>
+      <c r="G20" s="122"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="124"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>16</v>
@@ -2991,10 +2991,10 @@
       <c r="F21" s="21">
         <v>100</v>
       </c>
-      <c r="G21" s="123"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="125"/>
+      <c r="G21" s="122"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="124"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
         <v>18</v>
@@ -3005,10 +3005,10 @@
       <c r="F22" s="21">
         <v>100</v>
       </c>
-      <c r="G22" s="123"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="125"/>
+      <c r="G22" s="122"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="124"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>19</v>
@@ -3019,10 +3019,10 @@
       <c r="F23" s="21">
         <v>100</v>
       </c>
-      <c r="G23" s="123"/>
-    </row>
-    <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="118"/>
+      <c r="G23" s="122"/>
+    </row>
+    <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="117"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13" t="s">
         <v>28</v>
@@ -3033,10 +3033,10 @@
       <c r="F24" s="14">
         <v>100</v>
       </c>
-      <c r="G24" s="123"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="119" t="s">
+      <c r="G24" s="122"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="118" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="10" t="s">
@@ -3051,10 +3051,10 @@
       <c r="F25" s="20">
         <v>100</v>
       </c>
-      <c r="G25" s="123"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="120"/>
+      <c r="G25" s="122"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="119"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
         <v>8</v>
@@ -3065,10 +3065,10 @@
       <c r="F26" s="17">
         <v>100</v>
       </c>
-      <c r="G26" s="123"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="120"/>
+      <c r="G26" s="122"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="119"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
         <v>16</v>
@@ -3079,10 +3079,10 @@
       <c r="F27" s="17">
         <v>100</v>
       </c>
-      <c r="G27" s="123"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="120"/>
+      <c r="G27" s="122"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="119"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
         <v>21</v>
@@ -3093,10 +3093,10 @@
       <c r="F28" s="17">
         <v>100</v>
       </c>
-      <c r="G28" s="123"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="120"/>
+      <c r="G28" s="122"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="119"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
         <v>22</v>
@@ -3107,10 +3107,10 @@
       <c r="F29" s="17">
         <v>100</v>
       </c>
-      <c r="G29" s="123"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="120"/>
+      <c r="G29" s="122"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="119"/>
       <c r="C30" s="3" t="s">
         <v>13</v>
       </c>
@@ -3123,10 +3123,10 @@
       <c r="F30" s="17">
         <v>100</v>
       </c>
-      <c r="G30" s="123"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="120"/>
+      <c r="G30" s="122"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="119"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
         <v>8</v>
@@ -3137,10 +3137,10 @@
       <c r="F31" s="17">
         <v>100</v>
       </c>
-      <c r="G31" s="123"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="120"/>
+      <c r="G31" s="122"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="119"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
         <v>16</v>
@@ -3151,10 +3151,10 @@
       <c r="F32" s="17">
         <v>100</v>
       </c>
-      <c r="G32" s="123"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="120"/>
+      <c r="G32" s="122"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="119"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
         <v>21</v>
@@ -3165,10 +3165,10 @@
       <c r="F33" s="17">
         <v>100</v>
       </c>
-      <c r="G33" s="123"/>
-    </row>
-    <row r="34" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="121"/>
+      <c r="G33" s="122"/>
+    </row>
+    <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="120"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18" t="s">
         <v>22</v>
@@ -3179,7 +3179,7 @@
       <c r="F34" s="19">
         <v>100</v>
       </c>
-      <c r="G34" s="124"/>
+      <c r="G34" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3201,19 +3201,19 @@
       <selection activeCell="B13" sqref="B13:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.109375" customWidth="1"/>
-    <col min="7" max="7" width="42.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>29</v>
       </c>
@@ -3234,297 +3234,297 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="132" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="131" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="134" t="s">
+      <c r="D3" s="133" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="123" t="s">
+      <c r="E3" s="122" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="123" t="s">
+      <c r="F3" s="122" t="s">
         <v>71</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="122" t="s">
+      <c r="H3" s="121" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="132"/>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="131"/>
       <c r="C4" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="132"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
       <c r="G4" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="123"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="132"/>
+      <c r="H4" s="122"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="131"/>
       <c r="C5" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="132"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="122"/>
       <c r="G5" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="123"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="132"/>
+      <c r="H5" s="122"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="131"/>
       <c r="C6" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="132"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
       <c r="G6" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="123"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="132"/>
+      <c r="H6" s="122"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="131"/>
       <c r="C7" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="132"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
       <c r="G7" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="123"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="132"/>
+      <c r="H7" s="122"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="131"/>
       <c r="C8" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="132"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="123"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
       <c r="G8" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="123"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="132"/>
+      <c r="H8" s="122"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="131"/>
       <c r="C9" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="132"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
       <c r="G9" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="123"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="132"/>
+      <c r="H9" s="122"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="131"/>
       <c r="C10" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="132"/>
-      <c r="E10" s="123"/>
-      <c r="F10" s="123"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
       <c r="G10" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="123"/>
-    </row>
-    <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="132"/>
+      <c r="H10" s="122"/>
+    </row>
+    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="131"/>
       <c r="C11" s="36"/>
-      <c r="D11" s="132"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="123"/>
+      <c r="D11" s="131"/>
+      <c r="E11" s="122"/>
+      <c r="F11" s="122"/>
       <c r="G11" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="H11" s="123"/>
-    </row>
-    <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="133"/>
-      <c r="D12" s="132"/>
-      <c r="E12" s="124"/>
-      <c r="F12" s="123"/>
+      <c r="H11" s="122"/>
+    </row>
+    <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="132"/>
+      <c r="D12" s="131"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="122"/>
       <c r="G12" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="H12" s="124"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="123"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="132"/>
-      <c r="E13" s="135" t="s">
+      <c r="D13" s="131"/>
+      <c r="E13" s="134" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="126" t="s">
+      <c r="F13" s="125" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="138" t="s">
+      <c r="H13" s="137" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="132"/>
-      <c r="E14" s="136"/>
-      <c r="F14" s="127"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="135"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="139"/>
-    </row>
-    <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H14" s="138"/>
+    </row>
+    <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="132"/>
-      <c r="E15" s="136"/>
-      <c r="F15" s="128"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="135"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="140"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H15" s="139"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="132"/>
-      <c r="E16" s="136"/>
-      <c r="F16" s="148" t="s">
+      <c r="D16" s="131"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="147" t="s">
         <v>62</v>
       </c>
       <c r="G16" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="141" t="s">
+      <c r="H16" s="140" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="132"/>
-      <c r="E17" s="136"/>
-      <c r="F17" s="149"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="135"/>
+      <c r="F17" s="148"/>
       <c r="G17" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="142"/>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H17" s="141"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="132"/>
-      <c r="E18" s="136"/>
-      <c r="F18" s="150"/>
+      <c r="D18" s="131"/>
+      <c r="E18" s="135"/>
+      <c r="F18" s="149"/>
       <c r="G18" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="H18" s="143"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H18" s="142"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="132"/>
-      <c r="E19" s="136"/>
-      <c r="F19" s="154" t="s">
+      <c r="D19" s="131"/>
+      <c r="E19" s="135"/>
+      <c r="F19" s="153" t="s">
         <v>65</v>
       </c>
       <c r="G19" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="129" t="s">
+      <c r="H19" s="128" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="33"/>
-      <c r="D20" s="132"/>
-      <c r="E20" s="136"/>
-      <c r="F20" s="155"/>
+      <c r="D20" s="131"/>
+      <c r="E20" s="135"/>
+      <c r="F20" s="154"/>
       <c r="G20" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="H20" s="130"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D21" s="132"/>
-      <c r="E21" s="136"/>
-      <c r="F21" s="156" t="s">
+      <c r="H20" s="129"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D21" s="131"/>
+      <c r="E21" s="135"/>
+      <c r="F21" s="155" t="s">
         <v>67</v>
       </c>
       <c r="G21" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="144" t="s">
+      <c r="H21" s="143" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D22" s="132"/>
-      <c r="E22" s="136"/>
-      <c r="F22" s="157"/>
+    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="131"/>
+      <c r="E22" s="135"/>
+      <c r="F22" s="156"/>
       <c r="G22" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="H22" s="145"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D23" s="132"/>
-      <c r="E23" s="136"/>
-      <c r="F23" s="151" t="s">
+      <c r="H22" s="144"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="131"/>
+      <c r="E23" s="135"/>
+      <c r="F23" s="150" t="s">
         <v>70</v>
       </c>
       <c r="G23" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="H23" s="146" t="s">
+      <c r="H23" s="145" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D24" s="132"/>
-      <c r="E24" s="136"/>
-      <c r="F24" s="152"/>
+    <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="131"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="151"/>
       <c r="G24" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="H24" s="147"/>
-    </row>
-    <row r="25" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D25" s="132"/>
-      <c r="E25" s="136"/>
-      <c r="F25" s="152"/>
+      <c r="H24" s="146"/>
+    </row>
+    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="131"/>
+      <c r="E25" s="135"/>
+      <c r="F25" s="151"/>
       <c r="G25" s="51" t="s">
         <v>74</v>
       </c>
@@ -3532,37 +3532,38 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D26" s="132"/>
-      <c r="E26" s="136"/>
-      <c r="F26" s="152"/>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="131"/>
+      <c r="E26" s="135"/>
+      <c r="F26" s="151"/>
       <c r="G26" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="H26" s="129" t="s">
+      <c r="H26" s="128" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D27" s="132"/>
-      <c r="E27" s="136"/>
-      <c r="F27" s="152"/>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="131"/>
+      <c r="E27" s="135"/>
+      <c r="F27" s="151"/>
       <c r="G27" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="H27" s="131"/>
-    </row>
-    <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D28" s="133"/>
-      <c r="E28" s="137"/>
-      <c r="F28" s="153"/>
+      <c r="H27" s="130"/>
+    </row>
+    <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="132"/>
+      <c r="E28" s="136"/>
+      <c r="F28" s="152"/>
       <c r="G28" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="H28" s="130"/>
+      <c r="H28" s="129"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F21:F22"/>
     <mergeCell ref="E3:E12"/>
     <mergeCell ref="F13:F15"/>
     <mergeCell ref="H19:H20"/>
@@ -3579,7 +3580,6 @@
     <mergeCell ref="F16:F18"/>
     <mergeCell ref="F23:F28"/>
     <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F21:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3594,17 +3594,17 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>29</v>
       </c>
@@ -3619,75 +3619,75 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="132" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="131" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="132" t="s">
+      <c r="D3" s="131" t="s">
         <v>47</v>
       </c>
       <c r="E3" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="129" t="s">
+      <c r="F3" s="128" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="132"/>
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="131"/>
       <c r="C4" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="132"/>
+      <c r="D4" s="131"/>
       <c r="E4" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="130"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="132"/>
+      <c r="F4" s="129"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="131"/>
       <c r="C5" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="132"/>
+      <c r="D5" s="131"/>
       <c r="E5" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="129" t="s">
+      <c r="F5" s="128" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="132"/>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="131"/>
       <c r="C6" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="132"/>
+      <c r="D6" s="131"/>
       <c r="E6" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="131"/>
-    </row>
-    <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="132"/>
+      <c r="F6" s="130"/>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="131"/>
       <c r="C7" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="132"/>
+      <c r="D7" s="131"/>
       <c r="E7" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="130"/>
-    </row>
-    <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="132"/>
+      <c r="F7" s="129"/>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="131"/>
       <c r="C8" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="132"/>
+      <c r="D8" s="131"/>
       <c r="E8" s="61" t="s">
         <v>87</v>
       </c>
@@ -3695,211 +3695,211 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="132"/>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="131"/>
       <c r="C9" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="132"/>
+      <c r="D9" s="131"/>
       <c r="E9" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="122" t="s">
+      <c r="F9" s="121" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="132"/>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="131"/>
       <c r="C10" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="132"/>
+      <c r="D10" s="131"/>
       <c r="E10" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="123"/>
-    </row>
-    <row r="11" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="132"/>
+      <c r="F10" s="122"/>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="131"/>
       <c r="C11" s="36"/>
-      <c r="D11" s="132"/>
+      <c r="D11" s="131"/>
       <c r="E11" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="F11" s="123"/>
-    </row>
-    <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="133"/>
-      <c r="D12" s="132"/>
+      <c r="F11" s="122"/>
+    </row>
+    <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="132"/>
+      <c r="D12" s="131"/>
       <c r="E12" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="F12" s="123"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F12" s="122"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="132"/>
+      <c r="D13" s="131"/>
       <c r="E13" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="F13" s="123"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F13" s="122"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="132"/>
+      <c r="D14" s="131"/>
       <c r="E14" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="123"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="122"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="132"/>
+      <c r="D15" s="131"/>
       <c r="E15" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="123"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F15" s="122"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="132"/>
+      <c r="D16" s="131"/>
       <c r="E16" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="123"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F16" s="122"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="132"/>
+      <c r="D17" s="131"/>
       <c r="E17" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="123"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="122"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="132"/>
+      <c r="D18" s="131"/>
       <c r="E18" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="123"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="122"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="132"/>
+      <c r="D19" s="131"/>
       <c r="E19" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="123"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F19" s="122"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="132"/>
+      <c r="D20" s="131"/>
       <c r="E20" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="F20" s="123"/>
-    </row>
-    <row r="21" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F20" s="122"/>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="33"/>
-      <c r="D21" s="132"/>
+      <c r="D21" s="131"/>
       <c r="E21" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="123"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D22" s="132"/>
+      <c r="F21" s="122"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="131"/>
       <c r="E22" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="F22" s="123"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D23" s="132"/>
+      <c r="F22" s="122"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="131"/>
       <c r="E23" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="123"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D24" s="132"/>
+      <c r="F23" s="122"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D24" s="131"/>
       <c r="E24" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="F24" s="123"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D25" s="132"/>
+      <c r="F24" s="122"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="131"/>
       <c r="E25" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="123"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D26" s="132"/>
+      <c r="F25" s="122"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D26" s="131"/>
       <c r="E26" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="F26" s="123"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D27" s="132"/>
+      <c r="F26" s="122"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="131"/>
       <c r="E27" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="F27" s="123"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D28" s="132"/>
+      <c r="F27" s="122"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="131"/>
       <c r="E28" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="F28" s="123"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D29" s="132"/>
+      <c r="F28" s="122"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D29" s="131"/>
       <c r="E29" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="123"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D30" s="132"/>
+      <c r="F29" s="122"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="131"/>
       <c r="E30" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="123"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D31" s="132"/>
+      <c r="F30" s="122"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D31" s="131"/>
       <c r="E31" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="123"/>
-    </row>
-    <row r="32" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D32" s="133"/>
+      <c r="F31" s="122"/>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="132"/>
       <c r="E32" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="F32" s="124"/>
+      <c r="F32" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3918,34 +3918,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T54"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.109375" style="64" customWidth="1"/>
-    <col min="2" max="2" width="3.88671875" style="64" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.44140625" style="64" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="64" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" style="64" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.77734375" style="64" customWidth="1"/>
-    <col min="7" max="7" width="3.6640625" style="64"/>
-    <col min="8" max="8" width="4.88671875" style="64" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" style="64" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" style="64" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="64" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" style="64" customWidth="1"/>
-    <col min="13" max="13" width="8.33203125" style="64" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" style="64" customWidth="1"/>
-    <col min="15" max="15" width="16.88671875" style="64" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" style="64" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.42578125" style="64" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="64" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="64" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="64" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" style="64"/>
+    <col min="8" max="8" width="4.85546875" style="64" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="64" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" style="64" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="64" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="64" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="64" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="64" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" style="64" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" style="64" customWidth="1"/>
-    <col min="17" max="17" width="13.5546875" style="64" customWidth="1"/>
-    <col min="18" max="20" width="14.6640625" style="64" customWidth="1"/>
-    <col min="21" max="16384" width="3.6640625" style="64"/>
+    <col min="17" max="17" width="13.5703125" style="64" customWidth="1"/>
+    <col min="18" max="20" width="14.7109375" style="64" customWidth="1"/>
+    <col min="21" max="16384" width="3.7109375" style="64"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="67" t="s">
         <v>115</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="71">
         <v>1</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="71">
         <v>2</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="71">
         <v>3</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="71">
         <v>4</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="71">
         <v>5</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="71">
         <v>6</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="67" t="s">
         <v>115</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="74">
         <v>7</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="74"/>
       <c r="C10" s="74"/>
       <c r="D10" s="74" t="s">
@@ -4262,7 +4262,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="74"/>
       <c r="C11" s="74"/>
       <c r="D11" s="74" t="s">
@@ -4291,7 +4291,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="74"/>
       <c r="C12" s="74"/>
       <c r="D12" s="74" t="s">
@@ -4320,7 +4320,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="74"/>
       <c r="C13" s="74"/>
       <c r="D13" s="74" t="s">
@@ -4352,7 +4352,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="74"/>
       <c r="C14" s="74"/>
       <c r="D14" s="74" t="s">
@@ -4381,7 +4381,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="74"/>
       <c r="C15" s="74"/>
       <c r="D15" s="74" t="s">
@@ -4410,7 +4410,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="74"/>
       <c r="C16" s="74"/>
       <c r="D16" s="74" t="s">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="E16" s="74"/>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="74"/>
       <c r="C17" s="74"/>
       <c r="D17" s="74" t="s">
@@ -4426,7 +4426,7 @@
       </c>
       <c r="E17" s="74"/>
     </row>
-    <row r="18" spans="2:20" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="74">
         <v>8</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="66"/>
       <c r="C19" s="66"/>
       <c r="D19" s="66"/>
@@ -4467,7 +4467,7 @@
       <c r="S19" s="77"/>
       <c r="T19" s="78"/>
     </row>
-    <row r="20" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="66"/>
       <c r="C20" s="66"/>
       <c r="D20" s="66"/>
@@ -4510,7 +4510,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="66"/>
       <c r="C21" s="66"/>
       <c r="D21" s="66"/>
@@ -4553,7 +4553,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="66"/>
       <c r="C22" s="66"/>
       <c r="D22" s="66"/>
@@ -4596,7 +4596,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="2:20" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:20" ht="60" x14ac:dyDescent="0.25">
       <c r="B23" s="66"/>
       <c r="C23" s="66"/>
       <c r="D23" s="66"/>
@@ -4639,7 +4639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="66"/>
       <c r="C24" s="66"/>
       <c r="D24" s="66"/>
@@ -4682,7 +4682,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:20" ht="90" x14ac:dyDescent="0.25">
       <c r="B25" s="66"/>
       <c r="C25" s="66"/>
       <c r="D25" s="66"/>
@@ -4719,7 +4719,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:20" ht="120" x14ac:dyDescent="0.25">
       <c r="B26" s="66"/>
       <c r="C26" s="66"/>
       <c r="D26" s="66"/>
@@ -4756,7 +4756,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:20" ht="90" x14ac:dyDescent="0.25">
       <c r="B27" s="66"/>
       <c r="C27" s="66"/>
       <c r="D27" s="66"/>
@@ -4793,7 +4793,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="66"/>
       <c r="C28" s="66"/>
       <c r="D28" s="66"/>
@@ -4830,7 +4830,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:20" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="66"/>
       <c r="C29" s="66"/>
       <c r="D29" s="66"/>
@@ -4849,7 +4849,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:20" ht="60" x14ac:dyDescent="0.25">
       <c r="B30" s="66"/>
       <c r="C30" s="66"/>
       <c r="D30" s="66"/>
@@ -4865,168 +4865,168 @@
         <v>254</v>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" s="66"/>
       <c r="C31" s="66"/>
       <c r="D31" s="66"/>
       <c r="E31" s="66"/>
       <c r="F31" s="66"/>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="66"/>
       <c r="C32" s="66"/>
       <c r="D32" s="66"/>
       <c r="E32" s="66"/>
       <c r="F32" s="66"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="66"/>
       <c r="C33" s="66"/>
       <c r="D33" s="66"/>
       <c r="E33" s="66"/>
       <c r="F33" s="66"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="66"/>
       <c r="C34" s="66"/>
       <c r="D34" s="66"/>
       <c r="E34" s="66"/>
       <c r="F34" s="66"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="66"/>
       <c r="C35" s="66"/>
       <c r="D35" s="66"/>
       <c r="E35" s="66"/>
       <c r="F35" s="66"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="66"/>
       <c r="C36" s="66"/>
       <c r="D36" s="66"/>
       <c r="E36" s="66"/>
       <c r="F36" s="66"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="66"/>
       <c r="C37" s="66"/>
       <c r="D37" s="66"/>
       <c r="E37" s="66"/>
       <c r="F37" s="66"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="66"/>
       <c r="C38" s="66"/>
       <c r="D38" s="66"/>
       <c r="E38" s="66"/>
       <c r="F38" s="66"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="66"/>
       <c r="C39" s="66"/>
       <c r="D39" s="66"/>
       <c r="E39" s="66"/>
       <c r="F39" s="66"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="66"/>
       <c r="C40" s="66"/>
       <c r="D40" s="66"/>
       <c r="E40" s="66"/>
       <c r="F40" s="66"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="66"/>
       <c r="C41" s="66"/>
       <c r="D41" s="66"/>
       <c r="E41" s="66"/>
       <c r="F41" s="66"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="66"/>
       <c r="C42" s="66"/>
       <c r="D42" s="66"/>
       <c r="E42" s="66"/>
       <c r="F42" s="66"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="66"/>
       <c r="C43" s="66"/>
       <c r="D43" s="66"/>
       <c r="E43" s="66"/>
       <c r="F43" s="66"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="66"/>
       <c r="C44" s="66"/>
       <c r="D44" s="66"/>
       <c r="E44" s="66"/>
       <c r="F44" s="66"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="66"/>
       <c r="C45" s="66"/>
       <c r="D45" s="66"/>
       <c r="E45" s="66"/>
       <c r="F45" s="66"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="66"/>
       <c r="C46" s="66"/>
       <c r="D46" s="66"/>
       <c r="E46" s="66"/>
       <c r="F46" s="66"/>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="66"/>
       <c r="C47" s="66"/>
       <c r="D47" s="66"/>
       <c r="E47" s="66"/>
       <c r="F47" s="66"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="66"/>
       <c r="C48" s="66"/>
       <c r="D48" s="66"/>
       <c r="E48" s="66"/>
       <c r="F48" s="66"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="66"/>
       <c r="C49" s="66"/>
       <c r="D49" s="66"/>
       <c r="E49" s="66"/>
       <c r="F49" s="66"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="66"/>
       <c r="C50" s="66"/>
       <c r="D50" s="66"/>
       <c r="E50" s="66"/>
       <c r="F50" s="66"/>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="66"/>
       <c r="C51" s="66"/>
       <c r="D51" s="66"/>
       <c r="E51" s="66"/>
       <c r="F51" s="66"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="66"/>
       <c r="C52" s="66"/>
       <c r="D52" s="66"/>
       <c r="E52" s="66"/>
       <c r="F52" s="66"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="66"/>
       <c r="C53" s="66"/>
       <c r="D53" s="66"/>
       <c r="E53" s="66"/>
       <c r="F53" s="66"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="66"/>
       <c r="C54" s="66"/>
       <c r="D54" s="66"/>
@@ -5049,150 +5049,140 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="100" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="100" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="100" customWidth="1"/>
-    <col min="4" max="4" width="31.88671875" style="100" customWidth="1"/>
-    <col min="5" max="5" width="32.5546875" style="100" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" style="100" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="100"/>
+    <col min="1" max="1" width="9.5703125" style="100" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="100" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="100" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" style="100" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" style="100" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" style="100" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="100"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="158" t="s">
+    <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="160" t="s">
         <v>255</v>
       </c>
-      <c r="B1" s="158" t="s">
+      <c r="B1" s="160" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="158" t="s">
+      <c r="C1" s="160" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="158" t="s">
+      <c r="D1" s="157" t="s">
         <v>256</v>
       </c>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-    </row>
-    <row r="2" spans="1:6" s="101" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="158"/>
-      <c r="B2" s="158"/>
-      <c r="C2" s="158"/>
-      <c r="D2" s="158"/>
-      <c r="E2" s="158"/>
-      <c r="F2" s="158"/>
-    </row>
-    <row r="3" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="159" t="s">
+      <c r="E1" s="157"/>
+      <c r="F1" s="157"/>
+    </row>
+    <row r="2" spans="1:6" ht="79.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="158" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="160" t="s">
+      <c r="B2" s="159" t="s">
         <v>257</v>
       </c>
-      <c r="C3" s="102" t="s">
+      <c r="C2" s="101" t="s">
         <v>258</v>
       </c>
-      <c r="D3" s="103" t="s">
+      <c r="D2" s="102" t="s">
         <v>259</v>
       </c>
-      <c r="E3" s="104" t="s">
+      <c r="E2" s="103" t="s">
         <v>260</v>
       </c>
-      <c r="F3" s="105"/>
-    </row>
-    <row r="4" spans="1:6" ht="182.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="159"/>
-      <c r="B4" s="160"/>
-      <c r="C4" s="106" t="s">
+      <c r="F2" s="104"/>
+    </row>
+    <row r="3" spans="1:6" ht="174.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="158"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="105" t="s">
         <v>261</v>
       </c>
-      <c r="D4" s="107" t="s">
+      <c r="D3" s="106" t="s">
         <v>262</v>
       </c>
-      <c r="E4" s="108" t="s">
+      <c r="E3" s="107" t="s">
         <v>263</v>
       </c>
-      <c r="F4" s="105"/>
-    </row>
-    <row r="5" spans="1:6" ht="126" x14ac:dyDescent="0.3">
-      <c r="A5" s="159"/>
-      <c r="B5" s="160"/>
-      <c r="C5" s="102" t="s">
+      <c r="F3" s="104"/>
+    </row>
+    <row r="4" spans="1:6" ht="120.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="158"/>
+      <c r="B4" s="159"/>
+      <c r="C4" s="101" t="s">
         <v>264</v>
       </c>
-      <c r="D5" s="109" t="s">
+      <c r="D4" s="108" t="s">
         <v>265</v>
       </c>
-      <c r="E5" s="110" t="s">
+      <c r="E4" s="109" t="s">
         <v>266</v>
       </c>
-      <c r="F5" s="109" t="s">
+      <c r="F4" s="108" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="99.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="159"/>
-      <c r="B6" s="160"/>
-      <c r="C6" s="106" t="s">
+    <row r="5" spans="1:6" ht="95.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="158"/>
+      <c r="B5" s="159"/>
+      <c r="C5" s="105" t="s">
         <v>268</v>
       </c>
-      <c r="D6" s="111" t="s">
+      <c r="D5" s="110" t="s">
         <v>269</v>
       </c>
-      <c r="E6" s="112" t="s">
+      <c r="E5" s="111" t="s">
         <v>270</v>
       </c>
-      <c r="F6" s="105"/>
-    </row>
-    <row r="7" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="113"/>
-    </row>
-    <row r="8" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="113"/>
-    </row>
-    <row r="9" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="113"/>
-    </row>
-    <row r="10" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="113"/>
-    </row>
-    <row r="11" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="113"/>
-    </row>
-    <row r="12" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="113"/>
-    </row>
-    <row r="13" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="113"/>
-    </row>
-    <row r="14" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="113"/>
-    </row>
-    <row r="15" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="113"/>
-    </row>
-    <row r="16" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="113"/>
-    </row>
-    <row r="17" spans="1:1" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="113"/>
+      <c r="F5" s="104"/>
+    </row>
+    <row r="6" spans="1:6" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="112"/>
+    </row>
+    <row r="7" spans="1:6" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="112"/>
+    </row>
+    <row r="8" spans="1:6" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="112"/>
+    </row>
+    <row r="9" spans="1:6" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="112"/>
+    </row>
+    <row r="10" spans="1:6" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="112"/>
+    </row>
+    <row r="11" spans="1:6" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="112"/>
+    </row>
+    <row r="12" spans="1:6" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="112"/>
+    </row>
+    <row r="13" spans="1:6" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="112"/>
+    </row>
+    <row r="14" spans="1:6" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="112"/>
+    </row>
+    <row r="15" spans="1:6" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="112"/>
+    </row>
+    <row r="16" spans="1:6" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="112"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:F2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B3:B6"/>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="D1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5206,18 +5196,18 @@
       <selection activeCell="B14" sqref="B7:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>121</v>
       </c>
@@ -5237,7 +5227,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>154</v>
       </c>
@@ -5254,7 +5244,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>156</v>
       </c>
@@ -5274,7 +5264,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>168</v>
       </c>
@@ -5294,7 +5284,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>161</v>
       </c>

</xml_diff>